<commit_message>
parameter updates, README fixes
</commit_message>
<xml_diff>
--- a/misc/parameters.xlsx
+++ b/misc/parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="0" windowWidth="19620" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="0" windowWidth="19840" windowHeight="12460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Parameter description</t>
   </si>
@@ -54,9 +54,6 @@
     <t>h_size</t>
   </si>
   <si>
-    <t>single-core streaming SVD</t>
-  </si>
-  <si>
     <t>single</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>This table indicates parameters that were varied for different data sets, or other important parameters that we just wanted to point out. Generally speaking, all other parameters were left as default values specified in function definitions (github SHA 57c012182709c47719f8b763658dfef139d95f69)</t>
+  </si>
+  <si>
+    <t>single-instance streaming SVD</t>
+  </si>
+  <si>
+    <t>Iterative LSA</t>
   </si>
 </sst>
 </file>
@@ -151,8 +154,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,11 +174,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
@@ -518,7 +529,7 @@
     <col min="7" max="7" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,10 +549,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -563,8 +577,11 @@
       <c r="G2" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -584,18 +601,21 @@
         <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>0</v>
@@ -609,16 +629,19 @@
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="2">
         <v>0.8</v>
@@ -632,16 +655,19 @@
       <c r="G5" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>0.6</v>
@@ -653,18 +679,21 @@
         <v>0.75</v>
       </c>
       <c r="G6" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>0.6</v>
@@ -676,38 +705,44 @@
         <v>0.75</v>
       </c>
       <c r="G7" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
README and parameters.xlsx updates
</commit_message>
<xml_diff>
--- a/misc/parameters.xlsx
+++ b/misc/parameters.xlsx
@@ -515,7 +515,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -604,7 +604,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9">

</xml_diff>